<commit_message>
processed top down to SDG-084
</commit_message>
<xml_diff>
--- a/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019_JN.xlsx
+++ b/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019_JN.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9330" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Offsets" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="ESRI_MAPINFO_SHEET" sheetId="4" state="veryHidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Clips!$A$1:$E$472</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Clips!$A$1:$E$475</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Data Deliverable Notes'!$A$1:$C$41</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Offsets!$A$1:$G$70</definedName>
   </definedNames>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="133">
   <si>
     <t>Site</t>
   </si>
@@ -382,25 +382,13 @@
     <t>Jn Completed?</t>
   </si>
   <si>
-    <t>lots of drop outs. Drop outs on previous deliverable not clipped</t>
-  </si>
-  <si>
     <t>debris- confirmed by game cam</t>
-  </si>
-  <si>
-    <t>Debris in weir 6/4- 6/7 on old deliverable not clipped. Several debris clips in July</t>
-  </si>
-  <si>
-    <t>Probe and battery failures</t>
   </si>
   <si>
     <t>removed probe to clean</t>
   </si>
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">some drop offs in </t>
   </si>
   <si>
     <t>Bad data-doesn't match with game cam</t>
@@ -412,13 +400,37 @@
     <t>level spike on 7/15 same day as manual download. Looks like pattern of higher water temp with the pumping pattern. One period of data (7/9-7/15) was clipped out since it didn't match up with the game cam observations</t>
   </si>
   <si>
-    <t>after May calibrations below data delivered by 0.5 gpm</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
     <t>erroneous data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">none </t>
+  </si>
+  <si>
+    <t>after May calibrations below data delivered by 0.5 gpm. ALTA data consistantly above wood data ~0.5 gpm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">high flow spike 7/23. Note on 8/1 of evidence of high flow </t>
+  </si>
+  <si>
+    <t>lots of data drop out for july. ALTA data generally below Wood data ~ 1gpm. Also, appears delay in wood data. Likely because ALTA probe  upstream of Wood probe</t>
+  </si>
+  <si>
+    <t>debris</t>
+  </si>
+  <si>
+    <t>lots of data drop outs for july. Debris in weir 7/9-7/12. ALTA data under estimating peaks and over estimating troughs</t>
+  </si>
+  <si>
+    <t>bad probe- replaced</t>
+  </si>
+  <si>
+    <t>battery failure</t>
+  </si>
+  <si>
+    <t>Battery failure 7/16-7/22. bad probe, replaced 7/31. Several debis issues</t>
   </si>
 </sst>
 </file>
@@ -2807,11 +2819,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:XFC1348"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A455" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D476" sqref="D476"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D477" sqref="D477"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2839,7 +2852,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -2854,7 +2867,7 @@
       </c>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2868,7 +2881,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -2882,7 +2895,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -2897,7 +2910,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
@@ -2911,7 +2924,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
@@ -2925,7 +2938,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>4</v>
       </c>
@@ -2939,7 +2952,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
@@ -2953,7 +2966,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>4</v>
       </c>
@@ -2968,7 +2981,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
@@ -2985,7 +2998,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -2999,7 +3012,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
@@ -3013,7 +3026,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -3027,7 +3040,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
@@ -3041,7 +3054,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
@@ -3055,7 +3068,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
@@ -3069,7 +3082,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
@@ -3083,7 +3096,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>5</v>
       </c>
@@ -3097,7 +3110,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
@@ -3111,7 +3124,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>5</v>
       </c>
@@ -3125,7 +3138,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
@@ -3139,7 +3152,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
@@ -3153,7 +3166,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
@@ -3167,7 +3180,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>29</v>
       </c>
@@ -3184,7 +3197,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>29</v>
       </c>
@@ -3201,7 +3214,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>29</v>
       </c>
@@ -3218,7 +3231,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
@@ -3235,7 +3248,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
@@ -3249,7 +3262,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
@@ -3263,7 +3276,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
@@ -3277,7 +3290,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>29</v>
       </c>
@@ -3291,7 +3304,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>24</v>
       </c>
@@ -3308,7 +3321,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>24</v>
       </c>
@@ -3325,7 +3338,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>24</v>
       </c>
@@ -3342,7 +3355,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>24</v>
       </c>
@@ -3359,7 +3372,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>24</v>
       </c>
@@ -3373,7 +3386,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>24</v>
       </c>
@@ -3387,7 +3400,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>24</v>
       </c>
@@ -3401,7 +3414,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>24</v>
       </c>
@@ -3415,7 +3428,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>24</v>
       </c>
@@ -3429,7 +3442,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>6</v>
       </c>
@@ -3443,7 +3456,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>6</v>
       </c>
@@ -3457,7 +3470,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>6</v>
       </c>
@@ -3471,7 +3484,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>6</v>
       </c>
@@ -3485,7 +3498,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>6</v>
       </c>
@@ -3499,7 +3512,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>6</v>
       </c>
@@ -3513,7 +3526,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>6</v>
       </c>
@@ -3527,7 +3540,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>7</v>
       </c>
@@ -3541,7 +3554,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>7</v>
       </c>
@@ -3555,7 +3568,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>7</v>
       </c>
@@ -3569,7 +3582,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>7</v>
       </c>
@@ -3583,7 +3596,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>7</v>
       </c>
@@ -3597,7 +3610,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>7</v>
       </c>
@@ -3612,7 +3625,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>7</v>
       </c>
@@ -3626,7 +3639,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>7</v>
       </c>
@@ -3640,7 +3653,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>7</v>
       </c>
@@ -3654,7 +3667,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>7</v>
       </c>
@@ -3668,7 +3681,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>7</v>
       </c>
@@ -3682,7 +3695,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>7</v>
       </c>
@@ -3696,7 +3709,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>7</v>
       </c>
@@ -3710,7 +3723,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>7</v>
       </c>
@@ -3724,7 +3737,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>7</v>
       </c>
@@ -3738,7 +3751,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>7</v>
       </c>
@@ -3752,7 +3765,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>7</v>
       </c>
@@ -3766,7 +3779,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="30" t="s">
         <v>7</v>
       </c>
@@ -3780,7 +3793,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>7</v>
       </c>
@@ -3794,7 +3807,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>7</v>
       </c>
@@ -3808,7 +3821,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="30" t="s">
         <v>7</v>
       </c>
@@ -3822,7 +3835,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>7</v>
       </c>
@@ -3836,7 +3849,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>7</v>
       </c>
@@ -3850,7 +3863,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="30" t="s">
         <v>7</v>
       </c>
@@ -3864,7 +3877,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>7</v>
       </c>
@@ -3878,7 +3891,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>7</v>
       </c>
@@ -3892,7 +3905,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="30" t="s">
         <v>7</v>
       </c>
@@ -3906,7 +3919,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>7</v>
       </c>
@@ -3920,7 +3933,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>7</v>
       </c>
@@ -3934,7 +3947,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="30" t="s">
         <v>7</v>
       </c>
@@ -3948,7 +3961,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>7</v>
       </c>
@@ -3962,7 +3975,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="30" t="s">
         <v>7</v>
       </c>
@@ -3976,7 +3989,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="81" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>7</v>
       </c>
@@ -3990,7 +4003,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="82" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="30" t="s">
         <v>7</v>
       </c>
@@ -4191,7 +4204,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>31</v>
       </c>
@@ -4205,7 +4218,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>31</v>
       </c>
@@ -4222,7 +4235,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>31</v>
       </c>
@@ -4237,7 +4250,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>31</v>
       </c>
@@ -4251,7 +4264,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="99" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>31</v>
       </c>
@@ -4265,7 +4278,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>49</v>
       </c>
@@ -4279,7 +4292,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>49</v>
       </c>
@@ -4293,7 +4306,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="102" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>49</v>
       </c>
@@ -4307,7 +4320,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="103" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>49</v>
       </c>
@@ -4321,7 +4334,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="104" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>49</v>
       </c>
@@ -4335,7 +4348,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>49</v>
       </c>
@@ -4349,7 +4362,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="106" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>49</v>
       </c>
@@ -4363,7 +4376,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="107" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>49</v>
       </c>
@@ -4377,7 +4390,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="108" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>49</v>
       </c>
@@ -4391,7 +4404,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="109" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>49</v>
       </c>
@@ -4405,7 +4418,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="110" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>49</v>
       </c>
@@ -4419,7 +4432,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="111" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>49</v>
       </c>
@@ -4433,7 +4446,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="112" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>49</v>
       </c>
@@ -4447,7 +4460,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>49</v>
       </c>
@@ -4461,7 +4474,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>49</v>
       </c>
@@ -4475,7 +4488,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="115" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>49</v>
       </c>
@@ -4489,7 +4502,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>49</v>
       </c>
@@ -4503,7 +4516,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>49</v>
       </c>
@@ -4517,7 +4530,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="118" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>49</v>
       </c>
@@ -4531,7 +4544,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="119" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>49</v>
       </c>
@@ -4542,10 +4555,10 @@
         <v>43648.541666666664</v>
       </c>
       <c r="D119" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>42</v>
       </c>
@@ -4562,7 +4575,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="121" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>42</v>
       </c>
@@ -4579,7 +4592,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>42</v>
       </c>
@@ -4596,7 +4609,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="123" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>42</v>
       </c>
@@ -4610,7 +4623,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="124" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>42</v>
       </c>
@@ -4624,7 +4637,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="125" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>42</v>
       </c>
@@ -4638,7 +4651,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="126" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>42</v>
       </c>
@@ -4652,7 +4665,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="127" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>42</v>
       </c>
@@ -4666,7 +4679,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="128" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>50</v>
       </c>
@@ -4683,7 +4696,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="129" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>50</v>
       </c>
@@ -4697,7 +4710,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>50</v>
       </c>
@@ -4711,7 +4724,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="131" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>50</v>
       </c>
@@ -4725,7 +4738,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="132" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>50</v>
       </c>
@@ -4739,7 +4752,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="133" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>50</v>
       </c>
@@ -4753,7 +4766,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="134" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>50</v>
       </c>
@@ -4767,7 +4780,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="135" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>50</v>
       </c>
@@ -4781,7 +4794,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="136" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>50</v>
       </c>
@@ -4795,7 +4808,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="137" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>50</v>
       </c>
@@ -4809,7 +4822,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="138" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>50</v>
       </c>
@@ -4823,7 +4836,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="139" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>50</v>
       </c>
@@ -4837,7 +4850,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="140" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>50</v>
       </c>
@@ -4851,7 +4864,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="141" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>50</v>
       </c>
@@ -4865,7 +4878,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="142" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>50</v>
       </c>
@@ -4879,7 +4892,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="143" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>8</v>
       </c>
@@ -4893,7 +4906,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="144" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>8</v>
       </c>
@@ -4907,7 +4920,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="145" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>8</v>
       </c>
@@ -4921,7 +4934,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="146" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>8</v>
       </c>
@@ -4935,7 +4948,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="147" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>8</v>
       </c>
@@ -4949,7 +4962,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="148" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>8</v>
       </c>
@@ -4963,7 +4976,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="149" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>8</v>
       </c>
@@ -4977,7 +4990,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="150" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>8</v>
       </c>
@@ -4991,7 +5004,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="151" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>8</v>
       </c>
@@ -5005,7 +5018,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="152" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>8</v>
       </c>
@@ -5019,7 +5032,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="153" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>8</v>
       </c>
@@ -5033,7 +5046,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="154" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>8</v>
       </c>
@@ -5047,7 +5060,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="155" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>9</v>
       </c>
@@ -5061,7 +5074,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="156" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>9</v>
       </c>
@@ -5075,7 +5088,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="157" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>9</v>
       </c>
@@ -5089,7 +5102,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="158" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
         <v>9</v>
       </c>
@@ -13293,7 +13306,7 @@
       <c r="XFB158" s="8"/>
       <c r="XFC158" s="8"/>
     </row>
-    <row r="159" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
         <v>9</v>
       </c>
@@ -13307,7 +13320,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="160" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>10</v>
       </c>
@@ -13322,7 +13335,7 @@
       </c>
       <c r="E160" s="7"/>
     </row>
-    <row r="161" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>10</v>
       </c>
@@ -13337,7 +13350,7 @@
       </c>
       <c r="E161"/>
     </row>
-    <row r="162" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>10</v>
       </c>
@@ -13351,7 +13364,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="163" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
         <v>10</v>
       </c>
@@ -13365,7 +13378,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="164" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>10</v>
       </c>
@@ -13379,7 +13392,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="165" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>10</v>
       </c>
@@ -13393,7 +13406,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="166" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>10</v>
       </c>
@@ -13407,7 +13420,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="167" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>10</v>
       </c>
@@ -13421,7 +13434,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="168" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>10</v>
       </c>
@@ -13435,7 +13448,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="169" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
         <v>10</v>
       </c>
@@ -13449,7 +13462,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
         <v>11</v>
       </c>
@@ -13464,7 +13477,7 @@
       </c>
       <c r="E170" s="7"/>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
         <v>11</v>
       </c>
@@ -13478,7 +13491,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="172" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
         <v>11</v>
       </c>
@@ -13493,7 +13506,7 @@
       </c>
       <c r="E172"/>
     </row>
-    <row r="173" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
         <v>11</v>
       </c>
@@ -13507,7 +13520,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="174" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
         <v>11</v>
       </c>
@@ -13521,7 +13534,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="175" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
         <v>11</v>
       </c>
@@ -13535,7 +13548,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="176" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
         <v>11</v>
       </c>
@@ -13549,7 +13562,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="177" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
         <v>11</v>
       </c>
@@ -13563,7 +13576,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="178" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
         <v>12</v>
       </c>
@@ -13577,7 +13590,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
         <v>12</v>
       </c>
@@ -13592,7 +13605,7 @@
       </c>
       <c r="E179" s="7"/>
     </row>
-    <row r="180" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
         <v>12</v>
       </c>
@@ -13607,7 +13620,7 @@
       </c>
       <c r="E180"/>
     </row>
-    <row r="181" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
         <v>12</v>
       </c>
@@ -13621,7 +13634,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="182" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
         <v>12</v>
       </c>
@@ -13635,7 +13648,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="183" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
         <v>12</v>
       </c>
@@ -13649,7 +13662,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="184" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
         <v>12</v>
       </c>
@@ -13663,7 +13676,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="185" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
         <v>12</v>
       </c>
@@ -13677,7 +13690,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="186" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
         <v>12</v>
       </c>
@@ -13691,7 +13704,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="187" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
         <v>12</v>
       </c>
@@ -13705,7 +13718,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
         <v>40</v>
       </c>
@@ -13720,7 +13733,7 @@
       </c>
       <c r="E188" s="7"/>
     </row>
-    <row r="189" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
         <v>40</v>
       </c>
@@ -13735,7 +13748,7 @@
       </c>
       <c r="E189"/>
     </row>
-    <row r="190" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
         <v>40</v>
       </c>
@@ -13749,7 +13762,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="191" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
         <v>40</v>
       </c>
@@ -13763,7 +13776,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="192" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
         <v>40</v>
       </c>
@@ -13777,7 +13790,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="193" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
         <v>40</v>
       </c>
@@ -13791,7 +13804,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="194" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
         <v>40</v>
       </c>
@@ -13805,7 +13818,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="195" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
         <v>40</v>
       </c>
@@ -13819,7 +13832,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="196" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
         <v>40</v>
       </c>
@@ -13833,7 +13846,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="197" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
         <v>40</v>
       </c>
@@ -13847,7 +13860,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
         <v>40</v>
       </c>
@@ -13862,7 +13875,7 @@
       </c>
       <c r="E198" s="7"/>
     </row>
-    <row r="199" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
         <v>40</v>
       </c>
@@ -13877,7 +13890,7 @@
       </c>
       <c r="E199"/>
     </row>
-    <row r="200" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
         <v>40</v>
       </c>
@@ -13891,7 +13904,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="201" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
         <v>40</v>
       </c>
@@ -13905,7 +13918,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="202" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
         <v>41</v>
       </c>
@@ -13919,7 +13932,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="203" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
         <v>41</v>
       </c>
@@ -13933,7 +13946,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="204" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
         <v>41</v>
       </c>
@@ -13947,7 +13960,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="205" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
         <v>41</v>
       </c>
@@ -13961,7 +13974,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="206" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
         <v>41</v>
       </c>
@@ -13975,7 +13988,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="207" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
         <v>41</v>
       </c>
@@ -13989,7 +14002,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
         <v>41</v>
       </c>
@@ -14004,7 +14017,7 @@
       </c>
       <c r="E208" s="7"/>
     </row>
-    <row r="209" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
         <v>41</v>
       </c>
@@ -14019,7 +14032,7 @@
       </c>
       <c r="E209"/>
     </row>
-    <row r="210" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
         <v>41</v>
       </c>
@@ -14033,7 +14046,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="211" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
         <v>41</v>
       </c>
@@ -14047,7 +14060,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="212" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
         <v>41</v>
       </c>
@@ -14061,7 +14074,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="213" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
         <v>41</v>
       </c>
@@ -14075,7 +14088,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="214" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
         <v>41</v>
       </c>
@@ -14089,7 +14102,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
         <v>41</v>
       </c>
@@ -14104,7 +14117,7 @@
       </c>
       <c r="E215" s="7"/>
     </row>
-    <row r="216" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
         <v>13</v>
       </c>
@@ -14119,7 +14132,7 @@
       </c>
       <c r="E216"/>
     </row>
-    <row r="217" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
         <v>13</v>
       </c>
@@ -14133,7 +14146,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="218" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
         <v>13</v>
       </c>
@@ -14147,7 +14160,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="219" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
         <v>13</v>
       </c>
@@ -14161,7 +14174,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="220" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
         <v>13</v>
       </c>
@@ -14175,7 +14188,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="221" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
         <v>13</v>
       </c>
@@ -14189,7 +14202,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="222" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
         <v>13</v>
       </c>
@@ -14203,7 +14216,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="223" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
         <v>27</v>
       </c>
@@ -14217,7 +14230,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="224" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
         <v>27</v>
       </c>
@@ -14231,7 +14244,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="225" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
         <v>27</v>
       </c>
@@ -14245,7 +14258,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
         <v>27</v>
       </c>
@@ -14260,7 +14273,7 @@
       </c>
       <c r="E226" s="7"/>
     </row>
-    <row r="227" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
         <v>27</v>
       </c>
@@ -14275,7 +14288,7 @@
       </c>
       <c r="E227"/>
     </row>
-    <row r="228" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
         <v>27</v>
       </c>
@@ -14289,7 +14302,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="229" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
         <v>27</v>
       </c>
@@ -14303,7 +14316,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="230" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
         <v>27</v>
       </c>
@@ -14317,7 +14330,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="231" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
         <v>27</v>
       </c>
@@ -14331,7 +14344,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="232" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
         <v>27</v>
       </c>
@@ -14345,7 +14358,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="233" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
         <v>27</v>
       </c>
@@ -14359,7 +14372,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="234" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
         <v>14</v>
       </c>
@@ -14373,7 +14386,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
         <v>14</v>
       </c>
@@ -14388,7 +14401,7 @@
       </c>
       <c r="E235" s="7"/>
     </row>
-    <row r="236" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="3" t="s">
         <v>14</v>
       </c>
@@ -14403,7 +14416,7 @@
       </c>
       <c r="E236"/>
     </row>
-    <row r="237" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="s">
         <v>14</v>
       </c>
@@ -14417,7 +14430,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="238" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="3" t="s">
         <v>14</v>
       </c>
@@ -14431,7 +14444,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="239" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="3" t="s">
         <v>14</v>
       </c>
@@ -14445,7 +14458,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="240" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="3" t="s">
         <v>14</v>
       </c>
@@ -14459,7 +14472,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="241" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="3" t="s">
         <v>14</v>
       </c>
@@ -14473,7 +14486,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="242" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
         <v>14</v>
       </c>
@@ -14487,7 +14500,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="243" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="3" t="s">
         <v>14</v>
       </c>
@@ -14501,7 +14514,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="3" t="s">
         <v>14</v>
       </c>
@@ -14516,7 +14529,7 @@
       </c>
       <c r="E244" s="7"/>
     </row>
-    <row r="245" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="3" t="s">
         <v>14</v>
       </c>
@@ -14531,7 +14544,7 @@
       </c>
       <c r="E245"/>
     </row>
-    <row r="246" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="3" t="s">
         <v>14</v>
       </c>
@@ -14545,7 +14558,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="247" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="3" t="s">
         <v>15</v>
       </c>
@@ -14559,7 +14572,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="248" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="3" t="s">
         <v>15</v>
       </c>
@@ -14573,7 +14586,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="249" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="3" t="s">
         <v>15</v>
       </c>
@@ -14587,7 +14600,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="250" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="3" t="s">
         <v>15</v>
       </c>
@@ -14601,7 +14614,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="251" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="3" t="s">
         <v>15</v>
       </c>
@@ -14615,7 +14628,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="252" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="3" t="s">
         <v>15</v>
       </c>
@@ -14629,7 +14642,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="3" t="s">
         <v>15</v>
       </c>
@@ -14644,7 +14657,7 @@
       </c>
       <c r="E253" s="7"/>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="3" t="s">
         <v>15</v>
       </c>
@@ -14658,7 +14671,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="255" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="3" t="s">
         <v>15</v>
       </c>
@@ -14673,7 +14686,7 @@
       </c>
       <c r="E255"/>
     </row>
-    <row r="256" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="3" t="s">
         <v>15</v>
       </c>
@@ -14687,7 +14700,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="257" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="3" t="s">
         <v>15</v>
       </c>
@@ -14701,7 +14714,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="258" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="3" t="s">
         <v>15</v>
       </c>
@@ -14715,7 +14728,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="3" t="s">
         <v>15</v>
       </c>
@@ -14730,7 +14743,7 @@
       </c>
       <c r="E259" s="7"/>
     </row>
-    <row r="260" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="3" t="s">
         <v>15</v>
       </c>
@@ -14745,7 +14758,7 @@
       </c>
       <c r="E260"/>
     </row>
-    <row r="261" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="3" t="s">
         <v>16</v>
       </c>
@@ -14759,7 +14772,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="262" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="3" t="s">
         <v>16</v>
       </c>
@@ -14773,7 +14786,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="263" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="3" t="s">
         <v>16</v>
       </c>
@@ -14787,7 +14800,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="264" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="3" t="s">
         <v>16</v>
       </c>
@@ -14801,7 +14814,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="265" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="3" t="s">
         <v>16</v>
       </c>
@@ -14815,7 +14828,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="266" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="3" t="s">
         <v>16</v>
       </c>
@@ -14829,7 +14842,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="3" t="s">
         <v>16</v>
       </c>
@@ -14844,7 +14857,7 @@
       </c>
       <c r="E267" s="7"/>
     </row>
-    <row r="268" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="3" t="s">
         <v>16</v>
       </c>
@@ -14859,7 +14872,7 @@
       </c>
       <c r="E268"/>
     </row>
-    <row r="269" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="3" t="s">
         <v>16</v>
       </c>
@@ -14873,7 +14886,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="270" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="3" t="s">
         <v>16</v>
       </c>
@@ -14884,7 +14897,7 @@
         <v>43635</v>
       </c>
     </row>
-    <row r="271" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="3" t="s">
         <v>16</v>
       </c>
@@ -14898,7 +14911,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="272" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="3" t="s">
         <v>32</v>
       </c>
@@ -14912,7 +14925,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="3" t="s">
         <v>32</v>
       </c>
@@ -14927,7 +14940,7 @@
       </c>
       <c r="E273" s="7"/>
     </row>
-    <row r="274" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="3" t="s">
         <v>32</v>
       </c>
@@ -14942,7 +14955,7 @@
       </c>
       <c r="E274"/>
     </row>
-    <row r="275" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="3" t="s">
         <v>32</v>
       </c>
@@ -14956,7 +14969,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="276" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="3" t="s">
         <v>32</v>
       </c>
@@ -14970,7 +14983,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="277" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="3" t="s">
         <v>32</v>
       </c>
@@ -14984,7 +14997,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="278" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="3" t="s">
         <v>32</v>
       </c>
@@ -14998,7 +15011,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="279" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="3" t="s">
         <v>32</v>
       </c>
@@ -15012,7 +15025,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="280" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="3" t="s">
         <v>32</v>
       </c>
@@ -15026,7 +15039,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="3" t="s">
         <v>32</v>
       </c>
@@ -15041,7 +15054,7 @@
       </c>
       <c r="E281" s="7"/>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="7" t="s">
         <v>17</v>
       </c>
@@ -15055,7 +15068,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="283" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="7" t="s">
         <v>17</v>
       </c>
@@ -15070,7 +15083,7 @@
       </c>
       <c r="E283"/>
     </row>
-    <row r="284" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="7" t="s">
         <v>17</v>
       </c>
@@ -15084,7 +15097,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="285" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="7" t="s">
         <v>17</v>
       </c>
@@ -15098,7 +15111,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="286" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="7" t="s">
         <v>17</v>
       </c>
@@ -15112,7 +15125,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="287" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="7" t="s">
         <v>17</v>
       </c>
@@ -15126,7 +15139,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="288" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="7" t="s">
         <v>17</v>
       </c>
@@ -15140,7 +15153,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="289" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="7" t="s">
         <v>17</v>
       </c>
@@ -15154,7 +15167,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="7" t="s">
         <v>17</v>
       </c>
@@ -15169,7 +15182,7 @@
       </c>
       <c r="E290" s="7"/>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="7" t="s">
         <v>17</v>
       </c>
@@ -15183,7 +15196,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="292" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="7" t="s">
         <v>17</v>
       </c>
@@ -15198,7 +15211,7 @@
       </c>
       <c r="E292"/>
     </row>
-    <row r="293" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="7" t="s">
         <v>17</v>
       </c>
@@ -15212,7 +15225,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="294" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="24" t="s">
         <v>33</v>
       </c>
@@ -15226,7 +15239,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="295" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="7" t="s">
         <v>33</v>
       </c>
@@ -15240,7 +15253,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="296" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="7" t="s">
         <v>33</v>
       </c>
@@ -15254,7 +15267,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="297" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="24" t="s">
         <v>33</v>
       </c>
@@ -15268,7 +15281,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="298" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="24" t="s">
         <v>33</v>
       </c>
@@ -15282,7 +15295,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="299" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="24" t="s">
         <v>33</v>
       </c>
@@ -15296,7 +15309,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="300" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="24" t="s">
         <v>33</v>
       </c>
@@ -15310,7 +15323,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="301" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="24" t="s">
         <v>33</v>
       </c>
@@ -15324,7 +15337,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="302" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="3" t="s">
         <v>34</v>
       </c>
@@ -15338,7 +15351,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="3" t="s">
         <v>34</v>
       </c>
@@ -15353,7 +15366,7 @@
       </c>
       <c r="E303" s="7"/>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="3" t="s">
         <v>34</v>
       </c>
@@ -15367,7 +15380,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="305" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="3" t="s">
         <v>34</v>
       </c>
@@ -15382,7 +15395,7 @@
       </c>
       <c r="E305"/>
     </row>
-    <row r="306" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="3" t="s">
         <v>34</v>
       </c>
@@ -15396,7 +15409,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="307" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="3" t="s">
         <v>34</v>
       </c>
@@ -15410,7 +15423,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="3" t="s">
         <v>34</v>
       </c>
@@ -15425,7 +15438,7 @@
       </c>
       <c r="E308" s="7"/>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="3" t="s">
         <v>34</v>
       </c>
@@ -15439,7 +15452,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="3" t="s">
         <v>34</v>
       </c>
@@ -15453,7 +15466,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="3" t="s">
         <v>34</v>
       </c>
@@ -15467,7 +15480,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="312" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="3" t="s">
         <v>34</v>
       </c>
@@ -15482,7 +15495,7 @@
       </c>
       <c r="E312"/>
     </row>
-    <row r="313" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="3" t="s">
         <v>35</v>
       </c>
@@ -15496,7 +15509,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="314" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="3" t="s">
         <v>35</v>
       </c>
@@ -15510,7 +15523,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="315" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="3" t="s">
         <v>35</v>
       </c>
@@ -15524,7 +15537,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="316" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="3" t="s">
         <v>35</v>
       </c>
@@ -15538,7 +15551,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="317" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="3" t="s">
         <v>35</v>
       </c>
@@ -15552,7 +15565,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="3" t="s">
         <v>35</v>
       </c>
@@ -15567,7 +15580,7 @@
       </c>
       <c r="E318" s="7"/>
     </row>
-    <row r="319" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" s="3" t="s">
         <v>35</v>
       </c>
@@ -15581,7 +15594,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="320" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="3" t="s">
         <v>35</v>
       </c>
@@ -15595,7 +15608,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="321" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="3" t="s">
         <v>35</v>
       </c>
@@ -15609,7 +15622,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="3" t="s">
         <v>35</v>
       </c>
@@ -15624,7 +15637,7 @@
       </c>
       <c r="E322" s="7"/>
     </row>
-    <row r="323" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" s="3" t="s">
         <v>35</v>
       </c>
@@ -15638,7 +15651,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="324" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" s="3" t="s">
         <v>35</v>
       </c>
@@ -15652,7 +15665,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="325" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="3" t="s">
         <v>35</v>
       </c>
@@ -15666,7 +15679,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="326" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" s="3" t="s">
         <v>36</v>
       </c>
@@ -15680,7 +15693,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="327" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" s="3" t="s">
         <v>36</v>
       </c>
@@ -15694,7 +15707,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="328" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="3" t="s">
         <v>36</v>
       </c>
@@ -15708,7 +15721,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="329" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="3" t="s">
         <v>36</v>
       </c>
@@ -15722,7 +15735,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="330" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" s="3" t="s">
         <v>36</v>
       </c>
@@ -15736,7 +15749,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="331" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" s="3" t="s">
         <v>36</v>
       </c>
@@ -15750,7 +15763,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="332" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" s="3" t="s">
         <v>36</v>
       </c>
@@ -15764,7 +15777,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" s="3" t="s">
         <v>36</v>
       </c>
@@ -15779,7 +15792,7 @@
       </c>
       <c r="E333" s="7"/>
     </row>
-    <row r="334" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" s="3" t="s">
         <v>36</v>
       </c>
@@ -15793,7 +15806,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" s="3" t="s">
         <v>36</v>
       </c>
@@ -15808,7 +15821,7 @@
       </c>
       <c r="E335" s="7"/>
     </row>
-    <row r="336" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" s="3" t="s">
         <v>36</v>
       </c>
@@ -15822,7 +15835,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="337" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="3" t="s">
         <v>36</v>
       </c>
@@ -15836,7 +15849,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="338" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" s="29" t="s">
         <v>37</v>
       </c>
@@ -28134,7 +28147,7 @@
       <c r="XFB338" s="8"/>
       <c r="XFC338" s="8"/>
     </row>
-    <row r="339" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" s="3" t="s">
         <v>37</v>
       </c>
@@ -28148,7 +28161,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="340" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" s="29" t="s">
         <v>37</v>
       </c>
@@ -28162,7 +28175,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="341" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" s="3" t="s">
         <v>37</v>
       </c>
@@ -28177,7 +28190,7 @@
       </c>
       <c r="E341" s="7"/>
     </row>
-    <row r="342" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" s="3" t="s">
         <v>37</v>
       </c>
@@ -28191,7 +28204,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="343" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" s="3" t="s">
         <v>37</v>
       </c>
@@ -28205,7 +28218,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="344" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="29" t="s">
         <v>37</v>
       </c>
@@ -28219,7 +28232,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="345" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" s="3" t="s">
         <v>37</v>
       </c>
@@ -28233,7 +28246,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="346" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="29" t="s">
         <v>37</v>
       </c>
@@ -28247,7 +28260,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="347" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" s="29" t="s">
         <v>37</v>
       </c>
@@ -28261,7 +28274,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="348" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="29" t="s">
         <v>37</v>
       </c>
@@ -28275,7 +28288,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="349" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="29" t="s">
         <v>37</v>
       </c>
@@ -28289,7 +28302,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="350" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" s="3" t="s">
         <v>37</v>
       </c>
@@ -28303,7 +28316,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="351" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" s="3" t="s">
         <v>37</v>
       </c>
@@ -28317,7 +28330,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="352" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" s="3" t="s">
         <v>37</v>
       </c>
@@ -28331,7 +28344,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" s="29" t="s">
         <v>38</v>
       </c>
@@ -28345,7 +28358,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="354" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" s="3" t="s">
         <v>38</v>
       </c>
@@ -28360,7 +28373,7 @@
       </c>
       <c r="E354"/>
     </row>
-    <row r="355" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" s="29" t="s">
         <v>38</v>
       </c>
@@ -28374,7 +28387,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="356" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" s="3" t="s">
         <v>38</v>
       </c>
@@ -28388,7 +28401,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="357" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" s="29" t="s">
         <v>38</v>
       </c>
@@ -28402,7 +28415,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" s="29" t="s">
         <v>38</v>
       </c>
@@ -28417,7 +28430,7 @@
       </c>
       <c r="E358" s="7"/>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" s="29" t="s">
         <v>38</v>
       </c>
@@ -28431,7 +28444,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" s="29" t="s">
         <v>38</v>
       </c>
@@ -28445,7 +28458,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" s="3" t="s">
         <v>38</v>
       </c>
@@ -28459,7 +28472,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" s="3" t="s">
         <v>38</v>
       </c>
@@ -28473,7 +28486,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="363" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" s="3" t="s">
         <v>38</v>
       </c>
@@ -28488,7 +28501,7 @@
       </c>
       <c r="E363"/>
     </row>
-    <row r="364" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" s="3" t="s">
         <v>38</v>
       </c>
@@ -28502,7 +28515,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="365" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" s="3" t="s">
         <v>39</v>
       </c>
@@ -28516,7 +28529,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" s="3" t="s">
         <v>39</v>
       </c>
@@ -28531,7 +28544,7 @@
       </c>
       <c r="E366" s="7"/>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" s="3" t="s">
         <v>39</v>
       </c>
@@ -28545,7 +28558,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" s="3" t="s">
         <v>39</v>
       </c>
@@ -28559,7 +28572,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" s="3" t="s">
         <v>39</v>
       </c>
@@ -28573,7 +28586,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" s="3" t="s">
         <v>44</v>
       </c>
@@ -28587,7 +28600,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" s="3" t="s">
         <v>44</v>
       </c>
@@ -28601,7 +28614,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" s="3" t="s">
         <v>44</v>
       </c>
@@ -28615,7 +28628,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" s="3" t="s">
         <v>44</v>
       </c>
@@ -28632,7 +28645,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" s="3" t="s">
         <v>44</v>
       </c>
@@ -28646,7 +28659,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" s="3" t="s">
         <v>44</v>
       </c>
@@ -28660,7 +28673,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" s="3" t="s">
         <v>44</v>
       </c>
@@ -28675,7 +28688,7 @@
       </c>
       <c r="E376" s="7"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" s="3" t="s">
         <v>45</v>
       </c>
@@ -28692,7 +28705,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" s="3" t="s">
         <v>45</v>
       </c>
@@ -28709,7 +28722,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" s="3" t="s">
         <v>45</v>
       </c>
@@ -28724,7 +28737,7 @@
       </c>
       <c r="E379" s="7"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" s="3" t="s">
         <v>45</v>
       </c>
@@ -28739,7 +28752,7 @@
       </c>
       <c r="E380" s="7"/>
     </row>
-    <row r="381" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" s="3" t="s">
         <v>45</v>
       </c>
@@ -28754,7 +28767,7 @@
       </c>
       <c r="E381" s="7"/>
     </row>
-    <row r="382" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" s="3" t="s">
         <v>45</v>
       </c>
@@ -28769,7 +28782,7 @@
       </c>
       <c r="E382" s="7"/>
     </row>
-    <row r="383" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" s="3" t="s">
         <v>45</v>
       </c>
@@ -28784,7 +28797,7 @@
       </c>
       <c r="E383" s="7"/>
     </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" s="3" t="s">
         <v>45</v>
       </c>
@@ -28799,7 +28812,7 @@
       </c>
       <c r="E384" s="7"/>
     </row>
-    <row r="385" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" s="3" t="s">
         <v>45</v>
       </c>
@@ -28814,7 +28827,7 @@
       </c>
       <c r="E385" s="7"/>
     </row>
-    <row r="386" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" s="3" t="s">
         <v>45</v>
       </c>
@@ -28829,7 +28842,7 @@
       </c>
       <c r="E386" s="7"/>
     </row>
-    <row r="387" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" s="3" t="s">
         <v>45</v>
       </c>
@@ -28846,7 +28859,7 @@
       <c r="F387" s="8"/>
       <c r="G387" s="8"/>
     </row>
-    <row r="388" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:7" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" s="3" t="s">
         <v>45</v>
       </c>
@@ -28862,7 +28875,7 @@
       <c r="F388" s="8"/>
       <c r="G388" s="8"/>
     </row>
-    <row r="389" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:7" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" s="3" t="s">
         <v>45</v>
       </c>
@@ -28873,12 +28886,12 @@
         <v>43644.21875</v>
       </c>
       <c r="D389" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F389" s="8"/>
       <c r="G389" s="8"/>
     </row>
-    <row r="390" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:7" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" s="3" t="s">
         <v>45</v>
       </c>
@@ -28889,15 +28902,15 @@
         <v>43647.489583333336</v>
       </c>
       <c r="D390" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E390" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F390" s="8"/>
       <c r="G390" s="8"/>
     </row>
-    <row r="391" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:7" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" s="3" t="s">
         <v>45</v>
       </c>
@@ -28908,15 +28921,15 @@
         <v>43661.5625</v>
       </c>
       <c r="D391" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E391" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F391" s="8"/>
       <c r="G391" s="8"/>
     </row>
-    <row r="392" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" s="3" t="s">
         <v>45</v>
       </c>
@@ -28931,7 +28944,7 @@
       </c>
       <c r="E392" s="7"/>
     </row>
-    <row r="393" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:7" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" s="8" t="s">
         <v>45</v>
       </c>
@@ -28942,20 +28955,20 @@
         <v>43669.243055555555</v>
       </c>
       <c r="D393" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="394" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="394" spans="1:7" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" s="3"/>
       <c r="B394" s="8"/>
       <c r="C394" s="8"/>
     </row>
-    <row r="395" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:7" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" s="3"/>
       <c r="B395" s="8"/>
       <c r="C395" s="8"/>
     </row>
-    <row r="396" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" s="3" t="s">
         <v>46</v>
       </c>
@@ -28970,7 +28983,7 @@
       </c>
       <c r="E396" s="7"/>
     </row>
-    <row r="397" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" s="3" t="s">
         <v>46</v>
       </c>
@@ -28985,7 +28998,7 @@
       </c>
       <c r="E397" s="7"/>
     </row>
-    <row r="398" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" s="3" t="s">
         <v>46</v>
       </c>
@@ -29000,7 +29013,7 @@
       </c>
       <c r="E398" s="7"/>
     </row>
-    <row r="399" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" s="3" t="s">
         <v>46</v>
       </c>
@@ -29015,7 +29028,7 @@
       </c>
       <c r="E399" s="7"/>
     </row>
-    <row r="400" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" s="3" t="s">
         <v>46</v>
       </c>
@@ -29030,7 +29043,7 @@
       </c>
       <c r="E400" s="7"/>
     </row>
-    <row r="401" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" s="3" t="s">
         <v>46</v>
       </c>
@@ -29045,7 +29058,7 @@
       </c>
       <c r="E401" s="7"/>
     </row>
-    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" s="3" t="s">
         <v>46</v>
       </c>
@@ -29057,7 +29070,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" s="3" t="s">
         <v>18</v>
       </c>
@@ -29072,7 +29085,7 @@
       </c>
       <c r="E403" s="7"/>
     </row>
-    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" s="3" t="s">
         <v>18</v>
       </c>
@@ -29087,7 +29100,7 @@
       </c>
       <c r="E404" s="7"/>
     </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" s="3" t="s">
         <v>18</v>
       </c>
@@ -29102,7 +29115,7 @@
       </c>
       <c r="E405" s="7"/>
     </row>
-    <row r="406" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" s="3" t="s">
         <v>18</v>
       </c>
@@ -29117,7 +29130,7 @@
       </c>
       <c r="E406" s="7"/>
     </row>
-    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" s="3" t="s">
         <v>18</v>
       </c>
@@ -29132,7 +29145,7 @@
       </c>
       <c r="E407" s="3"/>
     </row>
-    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" s="3" t="s">
         <v>18</v>
       </c>
@@ -29147,7 +29160,7 @@
       </c>
       <c r="E408" s="7"/>
     </row>
-    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" s="3" t="s">
         <v>18</v>
       </c>
@@ -29162,7 +29175,7 @@
       </c>
       <c r="E409" s="7"/>
     </row>
-    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" s="3" t="s">
         <v>18</v>
       </c>
@@ -29177,7 +29190,7 @@
       </c>
       <c r="E410" s="7"/>
     </row>
-    <row r="411" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" s="3" t="s">
         <v>18</v>
       </c>
@@ -29192,7 +29205,7 @@
       </c>
       <c r="E411" s="7"/>
     </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" s="7" t="s">
         <v>26</v>
       </c>
@@ -29207,7 +29220,7 @@
       </c>
       <c r="E412" s="7"/>
     </row>
-    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" s="7" t="s">
         <v>26</v>
       </c>
@@ -29222,7 +29235,7 @@
       </c>
       <c r="E413" s="7"/>
     </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" s="7" t="s">
         <v>26</v>
       </c>
@@ -29237,7 +29250,7 @@
       </c>
       <c r="E414" s="7"/>
     </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" s="3" t="s">
         <v>26</v>
       </c>
@@ -29252,7 +29265,7 @@
       </c>
       <c r="E415" s="7"/>
     </row>
-    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" s="3" t="s">
         <v>26</v>
       </c>
@@ -29267,7 +29280,7 @@
       </c>
       <c r="E416" s="7"/>
     </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" s="3" t="s">
         <v>26</v>
       </c>
@@ -29282,7 +29295,7 @@
       </c>
       <c r="E417" s="7"/>
     </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" s="3" t="s">
         <v>26</v>
       </c>
@@ -29297,7 +29310,7 @@
       </c>
       <c r="E418" s="7"/>
     </row>
-    <row r="419" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" s="3" t="s">
         <v>26</v>
       </c>
@@ -29312,7 +29325,7 @@
       </c>
       <c r="E419" s="7"/>
     </row>
-    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" s="3" t="s">
         <v>26</v>
       </c>
@@ -29327,7 +29340,7 @@
       </c>
       <c r="E420" s="7"/>
     </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" s="7" t="s">
         <v>19</v>
       </c>
@@ -29342,7 +29355,7 @@
       </c>
       <c r="E421" s="7"/>
     </row>
-    <row r="422" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" s="7" t="s">
         <v>19</v>
       </c>
@@ -29357,7 +29370,7 @@
       </c>
       <c r="E422" s="7"/>
     </row>
-    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" s="7" t="s">
         <v>19</v>
       </c>
@@ -29372,7 +29385,7 @@
       </c>
       <c r="E423" s="7"/>
     </row>
-    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" s="7" t="s">
         <v>19</v>
       </c>
@@ -29387,7 +29400,7 @@
       </c>
       <c r="E424" s="7"/>
     </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" s="7" t="s">
         <v>19</v>
       </c>
@@ -29402,7 +29415,7 @@
       </c>
       <c r="E425" s="7"/>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" s="7" t="s">
         <v>19</v>
       </c>
@@ -29417,7 +29430,7 @@
       </c>
       <c r="E426" s="7"/>
     </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427" s="7" t="s">
         <v>19</v>
       </c>
@@ -29432,7 +29445,7 @@
       </c>
       <c r="E427" s="7"/>
     </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" s="7" t="s">
         <v>19</v>
       </c>
@@ -29447,7 +29460,7 @@
       </c>
       <c r="E428" s="7"/>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" s="7" t="s">
         <v>20</v>
       </c>
@@ -29462,7 +29475,7 @@
       </c>
       <c r="E429" s="7"/>
     </row>
-    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" s="7" t="s">
         <v>20</v>
       </c>
@@ -29477,7 +29490,7 @@
       </c>
       <c r="E430" s="7"/>
     </row>
-    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431" s="7" t="s">
         <v>20</v>
       </c>
@@ -29492,7 +29505,7 @@
       </c>
       <c r="E431" s="7"/>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" s="7" t="s">
         <v>20</v>
       </c>
@@ -29507,7 +29520,7 @@
       </c>
       <c r="E432" s="7"/>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433" s="7" t="s">
         <v>20</v>
       </c>
@@ -29522,7 +29535,7 @@
       </c>
       <c r="E433" s="7"/>
     </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" s="7" t="s">
         <v>20</v>
       </c>
@@ -29537,7 +29550,7 @@
       </c>
       <c r="E434" s="7"/>
     </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" s="7" t="s">
         <v>20</v>
       </c>
@@ -29552,7 +29565,7 @@
       </c>
       <c r="E435" s="7"/>
     </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" s="7" t="s">
         <v>20</v>
       </c>
@@ -29567,7 +29580,7 @@
       </c>
       <c r="E436" s="7"/>
     </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437" s="7" t="s">
         <v>20</v>
       </c>
@@ -29582,7 +29595,7 @@
       </c>
       <c r="E437" s="7"/>
     </row>
-    <row r="438" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" s="7" t="s">
         <v>20</v>
       </c>
@@ -29597,7 +29610,7 @@
       </c>
       <c r="E438" s="7"/>
     </row>
-    <row r="439" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" s="7" t="s">
         <v>25</v>
       </c>
@@ -29612,7 +29625,7 @@
       </c>
       <c r="E439" s="7"/>
     </row>
-    <row r="440" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" s="7" t="s">
         <v>25</v>
       </c>
@@ -29627,7 +29640,7 @@
       </c>
       <c r="E440" s="7"/>
     </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441" s="7" t="s">
         <v>25</v>
       </c>
@@ -29642,7 +29655,7 @@
       </c>
       <c r="E441" s="7"/>
     </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" s="7" t="s">
         <v>25</v>
       </c>
@@ -29657,7 +29670,7 @@
       </c>
       <c r="E442" s="7"/>
     </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443" s="7" t="s">
         <v>25</v>
       </c>
@@ -29672,7 +29685,7 @@
       </c>
       <c r="E443" s="7"/>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" s="7" t="s">
         <v>25</v>
       </c>
@@ -29687,7 +29700,7 @@
       </c>
       <c r="E444" s="7"/>
     </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445" s="7" t="s">
         <v>25</v>
       </c>
@@ -29702,7 +29715,7 @@
       </c>
       <c r="E445" s="7"/>
     </row>
-    <row r="446" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446" s="7" t="s">
         <v>25</v>
       </c>
@@ -29717,7 +29730,7 @@
       </c>
       <c r="E446" s="7"/>
     </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447" s="7" t="s">
         <v>25</v>
       </c>
@@ -29732,7 +29745,7 @@
       </c>
       <c r="E447" s="7"/>
     </row>
-    <row r="448" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448" s="7" t="s">
         <v>25</v>
       </c>
@@ -29747,7 +29760,7 @@
       </c>
       <c r="E448" s="7"/>
     </row>
-    <row r="449" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449" s="7" t="s">
         <v>25</v>
       </c>
@@ -29762,7 +29775,7 @@
       </c>
       <c r="E449" s="7"/>
     </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A450" s="7" t="s">
         <v>25</v>
       </c>
@@ -29777,7 +29790,7 @@
       </c>
       <c r="E450" s="7"/>
     </row>
-    <row r="451" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A451" s="3" t="s">
         <v>7</v>
       </c>
@@ -29792,7 +29805,7 @@
       </c>
       <c r="E451" s="7"/>
     </row>
-    <row r="452" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>7</v>
       </c>
@@ -29806,7 +29819,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="453" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>7</v>
       </c>
@@ -29820,7 +29833,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="454" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>7</v>
       </c>
@@ -29834,7 +29847,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="455" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>7</v>
       </c>
@@ -29848,7 +29861,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="456" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>7</v>
       </c>
@@ -29862,7 +29875,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="457" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A457" s="3" t="s">
         <v>49</v>
       </c>
@@ -29873,10 +29886,10 @@
         <v>43651.916666666664</v>
       </c>
       <c r="D457" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="458" spans="1:5" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="458" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A458" s="3" t="s">
         <v>49</v>
       </c>
@@ -29887,7 +29900,7 @@
         <v>43671.9375</v>
       </c>
       <c r="D458" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="459" spans="1:5" x14ac:dyDescent="0.25">
@@ -29901,7 +29914,7 @@
         <v>43648.583333333336</v>
       </c>
       <c r="D459" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="460" spans="1:5" x14ac:dyDescent="0.25">
@@ -29915,7 +29928,7 @@
         <v>43657.770833333336</v>
       </c>
       <c r="D460" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="461" spans="1:5" x14ac:dyDescent="0.25">
@@ -29929,7 +29942,7 @@
         <v>43672.670138888891</v>
       </c>
       <c r="D461" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="462" spans="1:5" x14ac:dyDescent="0.25">
@@ -29940,25 +29953,15 @@
         <v>43662.652777777781</v>
       </c>
       <c r="C462" s="8">
-        <v>43662.694444444445</v>
+        <v>43668.5625</v>
       </c>
       <c r="D462" s="7" t="s">
-        <v>75</v>
+        <v>131</v>
       </c>
     </row>
     <row r="463" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A463" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B463" s="8">
-        <v>43668.541666666664</v>
-      </c>
-      <c r="C463" s="8">
-        <v>43668.5625</v>
-      </c>
-      <c r="D463" s="7" t="s">
-        <v>75</v>
-      </c>
+      <c r="A463" s="3"/>
+      <c r="D463" s="7"/>
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A464" s="3" t="s">
@@ -29968,13 +29971,13 @@
         <v>43676.263888888891</v>
       </c>
       <c r="C464" s="8">
-        <v>43676.305555555555</v>
+        <v>43678</v>
       </c>
       <c r="D464" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="465" spans="1:4" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465" s="3" t="s">
         <v>4</v>
       </c>
@@ -29985,10 +29988,10 @@
         <v>43647.659722222219</v>
       </c>
       <c r="D465" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="466" spans="1:4" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A466" s="3" t="s">
         <v>15</v>
       </c>
@@ -30002,7 +30005,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="467" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A467" s="3" t="s">
         <v>15</v>
       </c>
@@ -30016,7 +30019,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="468" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A468" s="3" t="s">
         <v>15</v>
       </c>
@@ -30030,7 +30033,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="469" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A469" s="3" t="s">
         <v>15</v>
       </c>
@@ -30044,7 +30047,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="470" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470" s="3" t="s">
         <v>15</v>
       </c>
@@ -30058,7 +30061,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="471" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A471" s="3" t="s">
         <v>15</v>
       </c>
@@ -30072,7 +30075,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="472" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A472" s="3" t="s">
         <v>15</v>
       </c>
@@ -30086,7 +30089,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="473" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A473" s="3" t="s">
         <v>29</v>
       </c>
@@ -30097,20 +30100,50 @@
         <v>43647.614583333336</v>
       </c>
       <c r="D473" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A474" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B474" s="8">
+        <v>43647.576388888891</v>
+      </c>
+      <c r="C474" s="8">
+        <v>43647.583333333336</v>
+      </c>
+      <c r="D474" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A475" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B475" s="8">
+        <v>43655.15625</v>
+      </c>
+      <c r="C475" s="8">
+        <v>43658.364583333336</v>
+      </c>
+      <c r="D475" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="474" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B474"/>
-      <c r="C474"/>
-    </row>
-    <row r="475" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B475"/>
-      <c r="C475"/>
-    </row>
     <row r="476" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B476"/>
-      <c r="C476"/>
+      <c r="A476" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B476" s="8">
+        <v>43674.84375</v>
+      </c>
+      <c r="C476" s="8">
+        <v>43676.263888888891</v>
+      </c>
+      <c r="D476" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B477"/>
@@ -33601,7 +33634,13 @@
       <c r="C1348"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E472"/>
+  <autoFilter ref="A1:E475">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="SDG-084"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:E443">
     <sortCondition ref="A2:A443"/>
     <sortCondition ref="B2:B443"/>
@@ -33618,11 +33657,11 @@
   </sheetPr>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E16:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -33660,10 +33699,10 @@
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="32" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33675,10 +33714,10 @@
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="32" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33690,10 +33729,10 @@
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="32" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33704,7 +33743,12 @@
         <v>90</v>
       </c>
       <c r="C5" s="11"/>
-      <c r="D5" s="32"/>
+      <c r="D5" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
@@ -33714,9 +33758,11 @@
         <v>90</v>
       </c>
       <c r="C6" s="11"/>
-      <c r="D6" s="32"/>
+      <c r="D6" s="32" t="s">
+        <v>118</v>
+      </c>
       <c r="E6" s="10" t="s">
-        <v>90</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33727,12 +33773,14 @@
         <v>87</v>
       </c>
       <c r="C7" s="11"/>
-      <c r="D7" s="32"/>
+      <c r="D7" s="32" t="s">
+        <v>118</v>
+      </c>
       <c r="E7" s="10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28" t="s">
         <v>28</v>
       </c>
@@ -33740,9 +33788,11 @@
         <v>89</v>
       </c>
       <c r="C8" s="11"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="10" t="s">
-        <v>119</v>
+      <c r="D8" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33764,9 +33814,6 @@
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="32"/>
-      <c r="E10" s="10" t="s">
-        <v>118</v>
-      </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
@@ -33807,9 +33854,6 @@
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="32"/>
-      <c r="E14" s="10" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
@@ -34014,7 +34058,7 @@
         <v>45</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="32"/>

</xml_diff>